<commit_message>
fix(supplier): improve export and import UI layout
</commit_message>
<xml_diff>
--- a/PWL_POS/public/template_supplier.xlsx
+++ b/PWL_POS/public/template_supplier.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\= KULIAH\SEMESTER 4\3. PRAK JOBSHEET\PWL25\Minggu8\PWL_POS\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\= KULIAH\SEMESTER 4\3. PRAK JOBSHEET\PWL25\PWL_POS\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9278552A-685F-4ADE-AE5A-3872697FDEE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1B0FED1-0407-45AE-9D0E-5FBF910AD805}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3368A3D7-8FC4-4C2E-A7E9-623ECD7EB09E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>supplier_kode</t>
   </si>
@@ -47,74 +47,29 @@
     <t>supplier_alamat</t>
   </si>
   <si>
-    <t>SP04</t>
-  </si>
-  <si>
-    <t>SP05</t>
-  </si>
-  <si>
-    <t>SP06</t>
-  </si>
-  <si>
-    <t>SP07</t>
-  </si>
-  <si>
-    <t>SP08</t>
-  </si>
-  <si>
-    <t>SP09</t>
-  </si>
-  <si>
-    <t>SP10</t>
-  </si>
-  <si>
-    <t>PT Sinar Mulia</t>
-  </si>
-  <si>
-    <t>PT Gemilang Abadi</t>
-  </si>
-  <si>
-    <t>Jl. Sudirman No. 20, Jakarta</t>
-  </si>
-  <si>
-    <t>Jl. Basuki Rahmat No. 12, Malang</t>
-  </si>
-  <si>
-    <t>Jl. Kartini No. 5, Semarang</t>
-  </si>
-  <si>
-    <t>Jl. Asia Afrika No. 15, Bandung</t>
-  </si>
-  <si>
-    <t>PT Cahaya Nusantara</t>
-  </si>
-  <si>
-    <t>PT Mega Persada</t>
-  </si>
-  <si>
-    <t>Jl. Merdeka No. 25, Bandung</t>
-  </si>
-  <si>
-    <t>PT Mitra Jaya</t>
-  </si>
-  <si>
-    <t>PT Gunung Emas</t>
-  </si>
-  <si>
-    <t>Jl. Ahmad Dahlan No. 9, Balikpapan</t>
-  </si>
-  <si>
-    <t>PT Andalas Persada</t>
-  </si>
-  <si>
-    <t>Jl. Hasanuddin No. 6, Makassar</t>
+    <t>no_telp</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>SP11</t>
+  </si>
+  <si>
+    <t>PT Paragon Technology and Innovation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jl. Ciledug Raya No 10, Jakarta </t>
+  </si>
+  <si>
+    <t>eminacosmetics@paragon.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,6 +81,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -148,14 +111,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -488,20 +455,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1705CA23-10EB-4590-AC18-93B6EB3AF2F5}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="2" max="2" width="36" customWidth="1"/>
     <col min="3" max="3" width="36.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -511,85 +480,34 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="D2" s="2">
+        <v>6287701123000</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{573B6AE7-BB42-4DDD-B802-CBD5DE7A4DA8}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>